<commit_message>
first upload on github
</commit_message>
<xml_diff>
--- a/attendance/attendance_register.xlsx
+++ b/attendance/attendance_register.xlsx
@@ -344,10 +344,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -357,13 +357,7 @@
         <v>13</v>
       </c>
       <c r="C1" t="n">
-        <v>14</v>
-      </c>
-      <c r="D1" t="n">
-        <v>15</v>
-      </c>
-      <c r="E1" t="n">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2">
@@ -372,16 +366,6 @@
           <t>aashish</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>present</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>present</t>
-        </is>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -396,6 +380,11 @@
           <t>bishal</t>
         </is>
       </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>present</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>